<commit_message>
adding inbound request logs and sys perm setup
</commit_message>
<xml_diff>
--- a/db/source/system_permissions.xlsx
+++ b/db/source/system_permissions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wrburgess/Projects/aaa/kc-tennis/db/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F32728C-D7A5-974F-BC33-7BD9C0F62CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58F068D-4933-6E48-873C-4BBD56016EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="660" windowWidth="37160" windowHeight="20780" activeTab="3" xr2:uid="{A7924D65-00DE-2544-9F97-E11FDD26EDD2}"/>
+    <workbookView xWindow="1080" yWindow="660" windowWidth="37160" windowHeight="20780" xr2:uid="{A7924D65-00DE-2544-9F97-E11FDD26EDD2}"/>
   </bookViews>
   <sheets>
     <sheet name="system_permissions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="53">
   <si>
     <t>Contact</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>wrburgess@gmail.com</t>
+  </si>
+  <si>
+    <t>copy</t>
   </si>
 </sst>
 </file>
@@ -1087,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6930FAF-2397-5948-B560-84F685BD8951}">
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2007,7 +2010,7 @@
         <v>8</v>
       </c>
       <c r="B83" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>15</v>
@@ -2015,10 +2018,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B84" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>15</v>
@@ -2029,7 +2032,7 @@
         <v>9</v>
       </c>
       <c r="B85" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>15</v>
@@ -2040,7 +2043,7 @@
         <v>9</v>
       </c>
       <c r="B86" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>15</v>
@@ -2051,7 +2054,7 @@
         <v>9</v>
       </c>
       <c r="B87" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>15</v>
@@ -2062,7 +2065,7 @@
         <v>9</v>
       </c>
       <c r="B88" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>15</v>
@@ -2073,7 +2076,7 @@
         <v>9</v>
       </c>
       <c r="B89" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>15</v>
@@ -2084,7 +2087,7 @@
         <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>15</v>
@@ -2095,7 +2098,7 @@
         <v>9</v>
       </c>
       <c r="B91" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>15</v>
@@ -2106,7 +2109,7 @@
         <v>9</v>
       </c>
       <c r="B92" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>15</v>
@@ -2114,10 +2117,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B93" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>15</v>
@@ -2128,7 +2131,7 @@
         <v>10</v>
       </c>
       <c r="B94" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>15</v>
@@ -2139,7 +2142,7 @@
         <v>10</v>
       </c>
       <c r="B95" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>15</v>
@@ -2150,7 +2153,7 @@
         <v>10</v>
       </c>
       <c r="B96" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>15</v>
@@ -2161,7 +2164,7 @@
         <v>10</v>
       </c>
       <c r="B97" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>15</v>
@@ -2172,7 +2175,7 @@
         <v>10</v>
       </c>
       <c r="B98" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>15</v>
@@ -2183,7 +2186,7 @@
         <v>10</v>
       </c>
       <c r="B99" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>15</v>
@@ -2194,7 +2197,7 @@
         <v>10</v>
       </c>
       <c r="B100" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>15</v>
@@ -2205,7 +2208,7 @@
         <v>10</v>
       </c>
       <c r="B101" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>15</v>
@@ -2213,10 +2216,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B102" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>15</v>
@@ -2224,10 +2227,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="B103" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>15</v>
@@ -2238,7 +2241,7 @@
         <v>41</v>
       </c>
       <c r="B104" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>15</v>
@@ -2246,10 +2249,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B105" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>15</v>
@@ -2257,10 +2260,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B106" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>15</v>
@@ -2271,7 +2274,7 @@
         <v>4</v>
       </c>
       <c r="B107" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>15</v>
@@ -2282,7 +2285,7 @@
         <v>4</v>
       </c>
       <c r="B108" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>15</v>
@@ -2293,7 +2296,7 @@
         <v>4</v>
       </c>
       <c r="B109" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>15</v>
@@ -2304,7 +2307,7 @@
         <v>4</v>
       </c>
       <c r="B110" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>15</v>
@@ -2315,7 +2318,7 @@
         <v>4</v>
       </c>
       <c r="B111" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>15</v>
@@ -2326,7 +2329,7 @@
         <v>4</v>
       </c>
       <c r="B112" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>15</v>
@@ -2337,7 +2340,7 @@
         <v>4</v>
       </c>
       <c r="B113" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>15</v>
@@ -2348,9 +2351,20 @@
         <v>4</v>
       </c>
       <c r="B114" t="s">
+        <v>40</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>4</v>
+      </c>
+      <c r="B115" t="s">
         <v>39</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2533,7 +2547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2563C8-FCA3-B346-8303-FDE8EF30B49B}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>